<commit_message>
base de metas atualizada - versao final
</commit_message>
<xml_diff>
--- a/dados/saas/Base_Dados_SaaS_Metas.xlsx
+++ b/dados/saas/Base_Dados_SaaS_Metas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\data_analyst_altoqi\dados\saas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C560DEB0-0214-458F-B5DB-D73D734EC515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86947354-D519-4373-A276-C2EC712CF63F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>IdVendedor</t>
   </si>
@@ -388,11 +388,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3631"/>
+  <dimension ref="A1:C3631"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -400,7 +398,7 @@
     <col min="3" max="3" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -410,11 +408,8 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45292</v>
       </c>
@@ -424,11 +419,8 @@
       <c r="C2" s="2">
         <v>3314.001560623296</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45292</v>
       </c>
@@ -438,11 +430,8 @@
       <c r="C3" s="2">
         <v>20456.688473570513</v>
       </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45292</v>
       </c>
@@ -452,11 +441,8 @@
       <c r="C4" s="2">
         <v>11199.779927812911</v>
       </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45292</v>
       </c>
@@ -466,11 +452,8 @@
       <c r="C5" s="2">
         <v>26186.828962258413</v>
       </c>
-      <c r="H5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45292</v>
       </c>
@@ -480,11 +463,8 @@
       <c r="C6" s="2">
         <v>28226.719876886731</v>
       </c>
-      <c r="H6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45292</v>
       </c>
@@ -494,11 +474,8 @@
       <c r="C7" s="2">
         <v>7727.9808350892336</v>
       </c>
-      <c r="H7">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45292</v>
       </c>
@@ -508,11 +485,8 @@
       <c r="C8" s="2">
         <v>5270.8158212844637</v>
       </c>
-      <c r="H8">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45292</v>
       </c>
@@ -522,11 +496,8 @@
       <c r="C9" s="2">
         <v>2912.0686762371165</v>
       </c>
-      <c r="H9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45292</v>
       </c>
@@ -536,11 +507,8 @@
       <c r="C10" s="2">
         <v>15297.224517772351</v>
       </c>
-      <c r="H10">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45292</v>
       </c>
@@ -550,11 +518,8 @@
       <c r="C11" s="2">
         <v>7231.533278357595</v>
       </c>
-      <c r="H11">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45293</v>
       </c>
@@ -564,11 +529,8 @@
       <c r="C12" s="2">
         <v>4619.4223994602717</v>
       </c>
-      <c r="H12">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45293</v>
       </c>
@@ -579,7 +541,7 @@
         <v>4064.9057140066589</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45293</v>
       </c>
@@ -590,7 +552,7 @@
         <v>9906.0544049139698</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45293</v>
       </c>
@@ -601,7 +563,7 @@
         <v>12611.022853108449</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45293</v>
       </c>

</xml_diff>